<commit_message>
Adding and Updating new file
</commit_message>
<xml_diff>
--- a/TestData/OrangeHRMTestData.xlsx
+++ b/TestData/OrangeHRMTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adixit\PycharmProjects\RobotFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02664D91-B7AD-42A9-B0DB-9A7E8938AEB1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9969CD-D789-46A1-877B-A0F3AC24C6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>${username}</t>
   </si>
@@ -59,12 +59,18 @@
   </si>
   <si>
     <t>admin1234</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -315,11 +321,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -378,6 +384,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -385,7 +402,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -395,5 +412,6 @@
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>